<commit_message>
Updated XL sheet and parameters
</commit_message>
<xml_diff>
--- a/Retinal fundus images centres.xlsx
+++ b/Retinal fundus images centres.xlsx
@@ -6552,13 +6552,13 @@
         <v>257</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="G4" s="11" t="n">
-        <v>13.8924439894498</v>
+        <v>11.40175425099138</v>
       </c>
       <c r="H4" s="15" t="inlineStr">
         <is>
@@ -6580,13 +6580,13 @@
         <v>275</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G5" s="11" t="n">
-        <v>21.37755832643195</v>
+        <v>24.18677324489565</v>
       </c>
       <c r="H5" s="15" t="inlineStr">
         <is>
@@ -6611,14 +6611,14 @@
         <v>127</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="G6" s="11" t="n">
-        <v>37.16180835212409</v>
+        <v>34.0147027033899</v>
       </c>
       <c r="H6" s="15" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -6636,13 +6636,13 @@
         <v>275</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="G7" s="11" t="n">
-        <v>10.19803902718557</v>
+        <v>7.071067811865476</v>
       </c>
       <c r="H7" s="15" t="inlineStr">
         <is>
@@ -6664,13 +6664,13 @@
         <v>260</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="G8" s="11" t="n">
-        <v>13.0384048104053</v>
+        <v>18</v>
       </c>
       <c r="H8" s="15" t="inlineStr">
         <is>
@@ -6692,13 +6692,13 @@
         <v>270</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="G9" s="11" t="n">
-        <v>18.35755975068582</v>
+        <v>18.43908891458577</v>
       </c>
       <c r="H9" s="15" t="inlineStr">
         <is>
@@ -6720,13 +6720,13 @@
         <v>288</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="F10" s="5" t="n">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="G10" s="11" t="n">
-        <v>22.13594362117865</v>
+        <v>31.14482300479487</v>
       </c>
       <c r="H10" s="15" t="inlineStr">
         <is>
@@ -6748,13 +6748,13 @@
         <v>278</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="G11" s="11" t="n">
-        <v>30.06659275674582</v>
+        <v>33.37663853655727</v>
       </c>
       <c r="H11" s="15" t="inlineStr">
         <is>
@@ -6776,13 +6776,13 @@
         <v>270</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="G12" s="11" t="n">
-        <v>6.082762530298219</v>
+        <v>13.60147050873544</v>
       </c>
       <c r="H12" s="15" t="inlineStr">
         <is>
@@ -6804,13 +6804,13 @@
         <v>278</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>441</v>
+        <v>450</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="G13" s="11" t="n">
-        <v>31.90611226708763</v>
+        <v>18.97366596101028</v>
       </c>
       <c r="H13" s="15" t="inlineStr">
         <is>
@@ -6832,13 +6832,13 @@
         <v>270</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G14" s="11" t="n">
-        <v>9.848857801796104</v>
+        <v>11.31370849898476</v>
       </c>
       <c r="H14" s="15" t="inlineStr">
         <is>
@@ -6860,13 +6860,13 @@
         <v>260</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F15" s="5" t="n">
         <v>264</v>
       </c>
       <c r="G15" s="11" t="n">
-        <v>17.46424919657298</v>
+        <v>22.3606797749979</v>
       </c>
       <c r="H15" s="15" t="inlineStr">
         <is>
@@ -6888,13 +6888,13 @@
         <v>275</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="F16" s="5" t="n">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="G16" s="11" t="n">
-        <v>22.20360331117452</v>
+        <v>9.055385138137417</v>
       </c>
       <c r="H16" s="15" t="inlineStr">
         <is>
@@ -6916,13 +6916,13 @@
         <v>280</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="F17" s="5" t="n">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G17" s="5" t="n">
-        <v>7</v>
+        <v>22.02271554554524</v>
       </c>
       <c r="H17" s="15" t="inlineStr">
         <is>
@@ -6944,13 +6944,13 @@
         <v>280</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="F18" s="5" t="n">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G18" s="5" t="n">
-        <v>8</v>
+        <v>15.23154621172782</v>
       </c>
       <c r="H18" s="15" t="inlineStr">
         <is>
@@ -6972,13 +6972,13 @@
         <v>260</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="F19" s="5" t="n">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G19" s="11" t="n">
-        <v>9.219544457292887</v>
+        <v>19.23538406167134</v>
       </c>
       <c r="H19" s="15" t="inlineStr">
         <is>
@@ -7000,13 +7000,13 @@
         <v>265</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="F20" s="5" t="n">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="G20" s="11" t="n">
-        <v>23.53720459187964</v>
+        <v>21.37755832643195</v>
       </c>
       <c r="H20" s="15" t="inlineStr">
         <is>
@@ -7028,13 +7028,13 @@
         <v>260</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F21" s="5" t="n">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="G21" s="11" t="n">
-        <v>29.20616373302047</v>
+        <v>25.17935662402834</v>
       </c>
       <c r="H21" s="15" t="inlineStr">
         <is>
@@ -7056,13 +7056,13 @@
         <v>280</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F22" s="5" t="n">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G22" s="11" t="n">
-        <v>14.86606874731851</v>
+        <v>14.42220510185596</v>
       </c>
       <c r="H22" s="15" t="inlineStr">
         <is>
@@ -7084,13 +7084,13 @@
         <v>280</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="F23" s="5" t="n">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="G23" s="11" t="n">
-        <v>12.72792206135786</v>
+        <v>7.211102550927978</v>
       </c>
       <c r="H23" s="15" t="inlineStr">
         <is>
@@ -7112,13 +7112,13 @@
         <v>250</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="F24" s="5" t="n">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G24" s="5" t="n">
-        <v>5</v>
+        <v>12.52996408614167</v>
       </c>
       <c r="H24" s="15" t="inlineStr">
         <is>
@@ -7140,13 +7140,13 @@
         <v>275</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="F25" s="5" t="n">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="G25" s="11" t="n">
-        <v>21.93171219946131</v>
+        <v>16.15549442140351</v>
       </c>
       <c r="H25" s="15" t="inlineStr">
         <is>
@@ -7168,13 +7168,13 @@
         <v>225</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="F26" s="5" t="n">
-        <v>298</v>
+        <v>218</v>
       </c>
       <c r="G26" s="11" t="n">
-        <v>441.0827586746052</v>
+        <v>379.0646382874562</v>
       </c>
       <c r="H26" s="15" t="inlineStr">
         <is>
@@ -7196,13 +7196,13 @@
         <v>290</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="F27" s="5" t="n">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="G27" s="11" t="n">
-        <v>25.23885892824793</v>
+        <v>16.76305461424021</v>
       </c>
       <c r="H27" s="15" t="inlineStr">
         <is>
@@ -7224,13 +7224,13 @@
         <v>275</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>456</v>
+        <v>445</v>
       </c>
       <c r="F28" s="5" t="n">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="G28" s="5" t="n">
-        <v>15</v>
+        <v>20.09975124224178</v>
       </c>
       <c r="H28" s="15" t="inlineStr">
         <is>
@@ -7252,13 +7252,13 @@
         <v>250</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F29" s="5" t="n">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="G29" s="11" t="n">
-        <v>8.246211251235321</v>
+        <v>15.03329637837291</v>
       </c>
       <c r="H29" s="15" t="inlineStr">
         <is>
@@ -7280,13 +7280,13 @@
         <v>280</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="F30" s="5" t="n">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="G30" s="11" t="n">
-        <v>4.47213595499958</v>
+        <v>12.72792206135786</v>
       </c>
       <c r="H30" s="15" t="inlineStr">
         <is>
@@ -7308,13 +7308,13 @@
         <v>270</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>466</v>
+        <v>475</v>
       </c>
       <c r="F31" s="5" t="n">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="G31" s="11" t="n">
-        <v>24.02082429892863</v>
+        <v>15.03329637837291</v>
       </c>
       <c r="H31" s="15" t="inlineStr">
         <is>
@@ -7336,13 +7336,13 @@
         <v>270</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="F32" s="5" t="n">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="G32" s="11" t="n">
-        <v>29.1547594742265</v>
+        <v>16.97056274847714</v>
       </c>
       <c r="H32" s="15" t="inlineStr">
         <is>
@@ -7364,13 +7364,13 @@
         <v>290</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>482</v>
+        <v>470</v>
       </c>
       <c r="F33" s="5" t="n">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G33" s="11" t="n">
-        <v>8.062257748298549</v>
+        <v>20.8806130178211</v>
       </c>
       <c r="H33" s="15" t="inlineStr">
         <is>
@@ -7392,13 +7392,13 @@
         <v>250</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F34" s="5" t="n">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="G34" s="11" t="n">
-        <v>30.4138126514911</v>
+        <v>33.30165161069343</v>
       </c>
       <c r="H34" s="15" t="inlineStr">
         <is>
@@ -7420,13 +7420,13 @@
         <v>290</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>456</v>
+        <v>477</v>
       </c>
       <c r="F35" s="5" t="n">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G35" s="11" t="n">
-        <v>34.05877273185281</v>
+        <v>13.15294643796591</v>
       </c>
       <c r="H35" s="15" t="inlineStr">
         <is>
@@ -7448,13 +7448,13 @@
         <v>305</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="F36" s="5" t="n">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G36" s="11" t="n">
-        <v>14.42220510185596</v>
+        <v>21.02379604162864</v>
       </c>
       <c r="H36" s="15" t="inlineStr">
         <is>
@@ -7476,13 +7476,13 @@
         <v>230</v>
       </c>
       <c r="E37" s="13" t="n">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F37" s="13" t="n">
         <v>248</v>
       </c>
       <c r="G37" s="14" t="n">
-        <v>123.320720075744</v>
+        <v>126.2893503031827</v>
       </c>
       <c r="H37" s="12" t="inlineStr">
         <is>
@@ -7504,17 +7504,17 @@
         <v>280</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="F38" s="5" t="n">
-        <v>201</v>
+        <v>274</v>
       </c>
       <c r="G38" s="11" t="n">
-        <v>95.69221493935649</v>
+        <v>9.219544457292887</v>
       </c>
       <c r="H38" s="15" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -7532,13 +7532,13 @@
         <v>280</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>470</v>
+        <v>452</v>
       </c>
       <c r="F39" s="5" t="n">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="G39" s="5" t="n">
-        <v>7</v>
+        <v>19.69771560359221</v>
       </c>
       <c r="H39" s="15" t="inlineStr">
         <is>
@@ -7560,13 +7560,13 @@
         <v>290</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="F40" s="5" t="n">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="G40" s="5" t="n">
-        <v>10</v>
+        <v>17.20465053408525</v>
       </c>
       <c r="H40" s="15" t="inlineStr">
         <is>
@@ -7588,13 +7588,13 @@
         <v>275</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="F41" s="5" t="n">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="G41" s="11" t="n">
-        <v>13.15294643796591</v>
+        <v>8.602325267042627</v>
       </c>
       <c r="H41" s="15" t="inlineStr">
         <is>
@@ -7616,17 +7616,17 @@
         <v>265</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="F42" s="5" t="n">
-        <v>200</v>
+        <v>253</v>
       </c>
       <c r="G42" s="11" t="n">
-        <v>79.05694150420949</v>
+        <v>25.94224354214569</v>
       </c>
       <c r="H42" s="15" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -7644,13 +7644,13 @@
         <v>275</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F43" s="5" t="n">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="G43" s="11" t="n">
-        <v>27.20294101747089</v>
+        <v>13.45362404707371</v>
       </c>
       <c r="H43" s="15" t="inlineStr">
         <is>

</xml_diff>